<commit_message>
more songs in the spreadsheet
</commit_message>
<xml_diff>
--- a/titles/songs.xlsx
+++ b/titles/songs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\pi\pi-stereo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\pi\pi-seeburg\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="songs" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="110">
   <si>
     <t>Artist</t>
   </si>
@@ -234,6 +234,126 @@
   </si>
   <si>
     <t>V1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>David Bowie</t>
+  </si>
+  <si>
+    <t>Space Oddity</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>Life On Mars</t>
+  </si>
+  <si>
+    <t>/music/David Bowie/Bowie_ The Singles 1969-1993 (Disc 1)/01 Space Oddity.wav</t>
+  </si>
+  <si>
+    <t>/music/David Bowie/Bowie_ The Singles 1969-1993 (Disc 1)/04 Life on Mars_.wav</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Starman</t>
+  </si>
+  <si>
+    <t>/music/David Bowie/Bowie_ The Singles 1969-1993 (Disc 1)/06 Starman.wav</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Fame</t>
+  </si>
+  <si>
+    <t>/music/David Bowie/Bowie_ The Singles 1969-1993 (Disc 1)/15 Fame.wav</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>Under Pressure</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Dancing in the Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/music/David Bowie/Bowie_ The Singles 1969-1993 (Disc 2)/08 Under Pressure [with Queen].wav </t>
+  </si>
+  <si>
+    <t>/music/David Bowie/Bowie_ The Singles 1969-1993 (Disc 2)/15 Dancing in the Street [with Mick Jagger].wav</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Dire Straits</t>
+  </si>
+  <si>
+    <t>Money For Nothing</t>
+  </si>
+  <si>
+    <t>/music/Dire Straits/Brothers In Arms/02 Money for Nothing.wav</t>
+  </si>
+  <si>
+    <t>On Every Street</t>
+  </si>
+  <si>
+    <t>/music/Dire Straits/On Every Street/02 On Every Street.wav</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Duran Duran</t>
+  </si>
+  <si>
+    <t>A View To A Kill</t>
+  </si>
+  <si>
+    <t>Hungry Like the Wolf</t>
+  </si>
+  <si>
+    <t>/music/Duran Duran/Greatest/07 Hungry Like The Wolf.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/music/Duran Duran/Greatest/03 A View To A Kill.wav  </t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Elton John</t>
+  </si>
+  <si>
+    <t>I'm Still Standing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/music/Elton John/Greatest Hits 1976-1986/01 I'm Still Standing.wav </t>
+  </si>
+  <si>
+    <t>Don't Go Breaking My Heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/music/Elton John/Greatest Hits 1976-1986/06 Don't Go Breaking My Heart.wav </t>
   </si>
 </sst>
 </file>
@@ -551,17 +671,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" customWidth="1"/>
+    <col min="4" max="4" width="110.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -858,6 +978,174 @@
         <v>58</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reorganized and filled out the song database
</commit_message>
<xml_diff>
--- a/titles/songs.xlsx
+++ b/titles/songs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="431">
   <si>
     <t>Artist</t>
   </si>
@@ -332,12 +332,6 @@
     <t>tone:10000</t>
   </si>
   <si>
-    <t>tone:15000</t>
-  </si>
-  <si>
-    <t>tone:33000</t>
-  </si>
-  <si>
     <t>Android Sock Hop</t>
   </si>
   <si>
@@ -995,9 +989,6 @@
     <t>/music/UB40/Promises And Lies/08 Now And Then.wav</t>
   </si>
   <si>
-    <t>Various Artists</t>
-  </si>
-  <si>
     <t>Venus</t>
   </si>
   <si>
@@ -1007,19 +998,325 @@
     <t>You Keep Me Hangin' On</t>
   </si>
   <si>
-    <t>The Loco-Motion</t>
-  </si>
-  <si>
-    <t>/music/Various Artists/The 80's Hot Dance Trax/01 Venus - Bananarama.wav</t>
-  </si>
-  <si>
-    <t>/music/Various Artists/The 80's Hot Dance Trax/02 Two Of Hearts - Stacey Q.wav</t>
-  </si>
-  <si>
-    <t>/music/Various Artists/The 80's Hot Dance Trax/09 The Loco-Motion - Kylie Minogue.wav</t>
-  </si>
-  <si>
-    <t>/music/Various Artists/The 80's Hot Dance Trax/06 You Keep Me Hangin' On - Kim Wilde.wav</t>
+    <t>Pandora</t>
+  </si>
+  <si>
+    <t>pandora:quickmix</t>
+  </si>
+  <si>
+    <t>80s</t>
+  </si>
+  <si>
+    <t>pandora:80s</t>
+  </si>
+  <si>
+    <t>Quick Mix</t>
+  </si>
+  <si>
+    <t>Bananarama</t>
+  </si>
+  <si>
+    <t>Cruel Summer</t>
+  </si>
+  <si>
+    <t>I Heard a Rumor</t>
+  </si>
+  <si>
+    <t>I Can't Help It</t>
+  </si>
+  <si>
+    <t>/music/Bananarama/30YearsOf/07 Bananarama - Venus.wav</t>
+  </si>
+  <si>
+    <t>/music/Bananarama/30YearsOf/05 Bananarama - Cruel Summer.wa</t>
+  </si>
+  <si>
+    <t>/music/Bananarama/30YearsOf/08 Bananarama - I Heard A Rumour.wav</t>
+  </si>
+  <si>
+    <t>/music/Bananarama/30YearsOf/10 Bananarama - I Can't Help It.wav</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>The Look of Love</t>
+  </si>
+  <si>
+    <t>Vanity Kills</t>
+  </si>
+  <si>
+    <t>/music/ABC/BestOf/01. The Look of Love.wav</t>
+  </si>
+  <si>
+    <t>/music/ABC/BestOf/15. Vanity Kills.wav</t>
+  </si>
+  <si>
+    <t>A-Ha</t>
+  </si>
+  <si>
+    <t>Take On Me</t>
+  </si>
+  <si>
+    <t>The Living Daylights</t>
+  </si>
+  <si>
+    <t>/music/A-Ha/Singles/01 Take On Me.wav</t>
+  </si>
+  <si>
+    <t>/music/A-Ha/Singles/08 - The Living Daylights.wav</t>
+  </si>
+  <si>
+    <t>Devo</t>
+  </si>
+  <si>
+    <t>Whip It</t>
+  </si>
+  <si>
+    <t>Freedom of Choice</t>
+  </si>
+  <si>
+    <t>/music/Devo/1980 - Freedom of Choice [2008 Remaster]/03. Whip It.wav</t>
+  </si>
+  <si>
+    <t>/music/Devo/1980 - Freedom of Choice [2008 Remaster]/06. Freedom of Choice.wav</t>
+  </si>
+  <si>
+    <t>Kim Wilde</t>
+  </si>
+  <si>
+    <t>Kids In America</t>
+  </si>
+  <si>
+    <t>Chequered Love</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>You Came</t>
+  </si>
+  <si>
+    <t>In My Life</t>
+  </si>
+  <si>
+    <t>/music/Kim Wilde/Singles/01-Kids In America.wav</t>
+  </si>
+  <si>
+    <t>/music/Kim Wilde/Singles/02-Chequered Love.wav</t>
+  </si>
+  <si>
+    <t>/music/Kim Wilde/Singles/04-Cambodia.wav</t>
+  </si>
+  <si>
+    <t>/music/Kim Wilde/Singles/10-You Keep Me Hangin' On.wav</t>
+  </si>
+  <si>
+    <t>/music/Kim Wilde/Singles/12-You Came.wav</t>
+  </si>
+  <si>
+    <t>/music/Kim Wilde/Singles/17-In My Life.wav</t>
+  </si>
+  <si>
+    <t>Stacey Q</t>
+  </si>
+  <si>
+    <t>Swing Out Sister</t>
+  </si>
+  <si>
+    <t>Breakout</t>
+  </si>
+  <si>
+    <t>Surrender</t>
+  </si>
+  <si>
+    <t>/music/Swing Out Sister/Ultimate_CD1/01. Breakout.wav</t>
+  </si>
+  <si>
+    <t>/music/Swing Out Sister/Ultimate_CD1/02. Surrender.wav</t>
+  </si>
+  <si>
+    <t>Wang Chung</t>
+  </si>
+  <si>
+    <t>Everybody Have Fun Tonight</t>
+  </si>
+  <si>
+    <t>Dance Hall Days</t>
+  </si>
+  <si>
+    <t>To Live And Die In LA</t>
+  </si>
+  <si>
+    <t>Space Junk</t>
+  </si>
+  <si>
+    <t>/music/Wang Chung/TheMilleniumCollection/01 - Everybody Have Fun Tonight.wav</t>
+  </si>
+  <si>
+    <t>/music/Wang Chung/TheMilleniumCollection/02 - Dance Hall Days.wav</t>
+  </si>
+  <si>
+    <t>/music/Wang Chung/TheMilleniumCollection/06 - To Live And Die In LA.wav</t>
+  </si>
+  <si>
+    <t>/music/Wang Chung/TheMilleniumCollection/11 - Space Junk.wav</t>
+  </si>
+  <si>
+    <t>Gloria Estefan</t>
+  </si>
+  <si>
+    <t>Jennifer Rush</t>
+  </si>
+  <si>
+    <t>Quarterflash</t>
+  </si>
+  <si>
+    <t>Fleetwood Mac</t>
+  </si>
+  <si>
+    <t>Lita Ford</t>
+  </si>
+  <si>
+    <t>Kirsty MacColl</t>
+  </si>
+  <si>
+    <t>Karla Devito</t>
+  </si>
+  <si>
+    <t>Cry Wolf</t>
+  </si>
+  <si>
+    <t>Lifelines</t>
+  </si>
+  <si>
+    <t>/music/A-Ha/Singles/06 - Cry Wolf.wav</t>
+  </si>
+  <si>
+    <t>/music/A-Ha/Singles/19 - Lifelines.wav</t>
+  </si>
+  <si>
+    <t>Posion Arrow</t>
+  </si>
+  <si>
+    <t>/music/ABC/BestOf/03. Poison Arrow.wav</t>
+  </si>
+  <si>
+    <t>King Without A Crow</t>
+  </si>
+  <si>
+    <t>/music/ABC/BestOf/12. King Without a Crown.wav</t>
+  </si>
+  <si>
+    <t>/music/Animotion/Obsession - The Best Of Animotion/05 Strange Behaviour.wa</t>
+  </si>
+  <si>
+    <t>Strange Behavior</t>
+  </si>
+  <si>
+    <t>I Want You</t>
+  </si>
+  <si>
+    <t>/music/Animotion/Obsession - The Best Of Animotion/03 I Want You.wav</t>
+  </si>
+  <si>
+    <t>Walking Down Your Street</t>
+  </si>
+  <si>
+    <t>Eternal Flame</t>
+  </si>
+  <si>
+    <t>/music/Bangles/Greatest Hits/06 Walking Down Your Street.wav</t>
+  </si>
+  <si>
+    <t>/music/Bangles/Greatest Hits/10 Eternal Flame.wav</t>
+  </si>
+  <si>
+    <t>Tusk</t>
+  </si>
+  <si>
+    <t>Don't Stop</t>
+  </si>
+  <si>
+    <t>/music/Fleetwood Mac/Greatest/11 Fleetwood Mac - Tusk.wav</t>
+  </si>
+  <si>
+    <t>/music/Fleetwood Mac/Greatest/02 Fleetwood Mac - Don't Stop.wav</t>
+  </si>
+  <si>
+    <t>Rhythm Is Gonna Get You</t>
+  </si>
+  <si>
+    <t>Everlasting Love</t>
+  </si>
+  <si>
+    <t>Conga</t>
+  </si>
+  <si>
+    <t>Hold Me, Thrill Me, Kiss Me</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD1/02 Rhythm Is Gonna Get You.wav</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD1/04 Everlasting Love (Video Version).wav</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD1/18 Conga.wav</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD2/15 - Gloria Estefan - Hold Me, Thrill Me, Kiss Me.wav</t>
+  </si>
+  <si>
+    <t>Ring of Ice</t>
+  </si>
+  <si>
+    <t>nofn</t>
+  </si>
+  <si>
+    <t>Is This a Cool World or What</t>
+  </si>
+  <si>
+    <t>Midnight Confessions</t>
+  </si>
+  <si>
+    <t>Free World</t>
+  </si>
+  <si>
+    <t>In These Shoes</t>
+  </si>
+  <si>
+    <t>Kiss Me Deadly</t>
+  </si>
+  <si>
+    <t>Under The Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/music/Lita Ford/Greatest/04-Kiss Me Deadly.wav </t>
+  </si>
+  <si>
+    <t>/music/Lita Ford/Greatest/07-Under The Gun.wav</t>
+  </si>
+  <si>
+    <t>Harden My Heart</t>
+  </si>
+  <si>
+    <t>Find Another Fool</t>
+  </si>
+  <si>
+    <t>/music/Quarterflash/GreatestHits/01. Harden My Heart - Quarterflash.wav</t>
+  </si>
+  <si>
+    <t>/music/Quarterflash/GreatestHits/02. Find Another Fool - Quarterflash.wav</t>
+  </si>
+  <si>
+    <t>Better Than Heaver</t>
+  </si>
+  <si>
+    <t>/music/Jennifer Rush/TheVeryBestOf1/[01] [Jennifer Rush] The Power Of Love (Special Edit Version - Previously Unreleased).wav</t>
+  </si>
+  <si>
+    <t>/music/Jennifer Rush/TheVeryBestOf1/[03] [Jennifer Rush] Ring Of Ice (Special Edit Version).wav</t>
   </si>
 </sst>
 </file>
@@ -1337,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,10 +1649,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1369,2042 +1666,2042 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>77</v>
+      </c>
+      <c r="D2">
+        <v>91.9</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="D3">
+        <v>94.5</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>77</v>
+      </c>
+      <c r="D4">
+        <v>96.1</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+        <v>77</v>
+      </c>
+      <c r="D5">
+        <v>99.1</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>324</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>328</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>324</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>326</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
+        <v>95</v>
+      </c>
+      <c r="D8">
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
+        <v>95</v>
+      </c>
+      <c r="D9">
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
+        <v>95</v>
+      </c>
+      <c r="D10">
+        <v>330</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
+        <v>95</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
+        <v>95</v>
+      </c>
+      <c r="D13">
+        <v>3300</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
+        <v>95</v>
+      </c>
+      <c r="D14">
+        <v>10000</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>342</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>343</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>342</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>344</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>342</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>386</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>342</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>387</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>337</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>338</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>337</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>339</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>337</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>390</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>337</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>392</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>396</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>397</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>329</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>321</v>
       </c>
       <c r="E37" t="s">
-        <v>133</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>329</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>330</v>
       </c>
       <c r="E38" t="s">
-        <v>134</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>329</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>331</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>329</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>332</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>398</v>
       </c>
       <c r="E43" t="s">
-        <v>147</v>
+        <v>400</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>399</v>
       </c>
       <c r="E44" t="s">
-        <v>148</v>
+        <v>401</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
         <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" t="s">
-        <v>150</v>
-      </c>
-      <c r="E46" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>151</v>
+        <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>155</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>152</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>10</v>
       </c>
       <c r="E49" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>161</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>162</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>164</v>
+        <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="E54" t="s">
-        <v>170</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>169</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>172</v>
+        <v>34</v>
       </c>
       <c r="D57" t="s">
-        <v>173</v>
+        <v>35</v>
       </c>
       <c r="E57" t="s">
-        <v>175</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>172</v>
+        <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>174</v>
+        <v>37</v>
       </c>
       <c r="E58" t="s">
-        <v>176</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
-        <v>178</v>
+        <v>40</v>
       </c>
       <c r="E59" t="s">
-        <v>181</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="E60" t="s">
-        <v>180</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C61" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="D61" t="s">
-        <v>182</v>
+        <v>44</v>
       </c>
       <c r="E61" t="s">
-        <v>184</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="E62" t="s">
-        <v>185</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C63" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D63" t="s">
-        <v>187</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
-        <v>191</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C64" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D64" t="s">
-        <v>188</v>
+        <v>51</v>
       </c>
       <c r="E64" t="s">
-        <v>192</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C65" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D65" t="s">
-        <v>189</v>
+        <v>54</v>
       </c>
       <c r="E65" t="s">
-        <v>194</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D66" t="s">
-        <v>190</v>
+        <v>56</v>
       </c>
       <c r="E66" t="s">
-        <v>193</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D68" t="s">
-        <v>195</v>
+        <v>58</v>
       </c>
       <c r="E68" t="s">
-        <v>197</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D69" t="s">
-        <v>196</v>
+        <v>59</v>
       </c>
       <c r="E69" t="s">
-        <v>198</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>186</v>
+        <v>347</v>
       </c>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>348</v>
       </c>
       <c r="E70" t="s">
-        <v>202</v>
+        <v>350</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>186</v>
+        <v>347</v>
       </c>
       <c r="D71" t="s">
-        <v>200</v>
+        <v>349</v>
       </c>
       <c r="E71" t="s">
-        <v>201</v>
+        <v>351</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>186</v>
+        <v>62</v>
       </c>
       <c r="D72" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
       <c r="E72" t="s">
-        <v>205</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>186</v>
+        <v>62</v>
       </c>
       <c r="D73" t="s">
-        <v>204</v>
+        <v>65</v>
       </c>
       <c r="E73" t="s">
-        <v>206</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>207</v>
+        <v>67</v>
       </c>
       <c r="D74" t="s">
-        <v>208</v>
+        <v>68</v>
       </c>
       <c r="E74" t="s">
-        <v>210</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C75" t="s">
-        <v>207</v>
+        <v>67</v>
       </c>
       <c r="D75" t="s">
-        <v>209</v>
+        <v>69</v>
       </c>
       <c r="E75" t="s">
-        <v>211</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C76" t="s">
-        <v>212</v>
+        <v>72</v>
       </c>
       <c r="D76" t="s">
-        <v>213</v>
+        <v>73</v>
       </c>
       <c r="E76" t="s">
-        <v>215</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>72</v>
       </c>
       <c r="D77" t="s">
-        <v>214</v>
+        <v>75</v>
       </c>
       <c r="E77" t="s">
-        <v>216</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C79" t="s">
-        <v>217</v>
+        <v>128</v>
       </c>
       <c r="D79" t="s">
-        <v>195</v>
+        <v>129</v>
       </c>
       <c r="E79" t="s">
-        <v>221</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C80" t="s">
-        <v>217</v>
+        <v>128</v>
       </c>
       <c r="D80" t="s">
-        <v>218</v>
+        <v>130</v>
       </c>
       <c r="E80" t="s">
-        <v>222</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C81" t="s">
-        <v>217</v>
+        <v>133</v>
       </c>
       <c r="D81" t="s">
-        <v>219</v>
+        <v>134</v>
       </c>
       <c r="E81" t="s">
-        <v>223</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>217</v>
+        <v>133</v>
       </c>
       <c r="D82" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="E82" t="s">
-        <v>224</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>133</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
       <c r="E83" t="s">
-        <v>228</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C84" t="s">
-        <v>225</v>
+        <v>133</v>
       </c>
       <c r="D84" t="s">
-        <v>227</v>
+        <v>141</v>
       </c>
       <c r="E84" t="s">
-        <v>229</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C85" t="s">
-        <v>230</v>
+        <v>382</v>
       </c>
       <c r="D85" t="s">
-        <v>231</v>
+        <v>402</v>
       </c>
       <c r="E85" t="s">
-        <v>235</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C86" t="s">
-        <v>230</v>
+        <v>382</v>
       </c>
       <c r="D86" t="s">
-        <v>232</v>
+        <v>403</v>
       </c>
       <c r="E86" t="s">
-        <v>236</v>
+        <v>405</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C87" t="s">
-        <v>230</v>
+        <v>142</v>
       </c>
       <c r="D87" t="s">
-        <v>233</v>
+        <v>143</v>
       </c>
       <c r="E87" t="s">
-        <v>237</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C88" t="s">
-        <v>230</v>
+        <v>142</v>
       </c>
       <c r="D88" t="s">
-        <v>234</v>
+        <v>144</v>
       </c>
       <c r="E88" t="s">
-        <v>238</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C90" t="s">
-        <v>239</v>
+        <v>379</v>
       </c>
       <c r="D90" t="s">
-        <v>240</v>
+        <v>406</v>
       </c>
       <c r="E90" t="s">
-        <v>242</v>
+        <v>410</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>239</v>
+        <v>379</v>
       </c>
       <c r="D91" t="s">
-        <v>241</v>
+        <v>407</v>
       </c>
       <c r="E91" t="s">
-        <v>243</v>
+        <v>411</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B92" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>244</v>
+        <v>379</v>
       </c>
       <c r="D92" t="s">
-        <v>245</v>
+        <v>408</v>
       </c>
       <c r="E92" t="s">
-        <v>249</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>244</v>
+        <v>379</v>
       </c>
       <c r="D93" t="s">
-        <v>246</v>
+        <v>409</v>
       </c>
       <c r="E93" t="s">
-        <v>250</v>
+        <v>413</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C94" t="s">
-        <v>244</v>
+        <v>147</v>
       </c>
       <c r="D94" t="s">
-        <v>247</v>
+        <v>148</v>
       </c>
       <c r="E94" t="s">
-        <v>251</v>
+        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>244</v>
+        <v>147</v>
       </c>
       <c r="D95" t="s">
-        <v>248</v>
+        <v>149</v>
       </c>
       <c r="E95" t="s">
-        <v>252</v>
+        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C96" t="s">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="D96" t="s">
-        <v>254</v>
+        <v>150</v>
       </c>
       <c r="E96" t="s">
-        <v>256</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C97" t="s">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="D97" t="s">
-        <v>255</v>
+        <v>151</v>
       </c>
       <c r="E97" t="s">
-        <v>257</v>
+        <v>155</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>156</v>
       </c>
       <c r="D98" t="s">
-        <v>259</v>
+        <v>157</v>
       </c>
       <c r="E98" t="s">
-        <v>261</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C99" t="s">
-        <v>258</v>
+        <v>156</v>
       </c>
       <c r="D99" t="s">
-        <v>260</v>
+        <v>158</v>
       </c>
       <c r="E99" t="s">
-        <v>262</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>263</v>
+        <v>161</v>
       </c>
       <c r="D101" t="s">
-        <v>264</v>
+        <v>162</v>
       </c>
       <c r="E101" t="s">
-        <v>267</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C102" t="s">
-        <v>263</v>
+        <v>161</v>
       </c>
       <c r="D102" t="s">
-        <v>265</v>
+        <v>163</v>
       </c>
       <c r="E102" t="s">
-        <v>266</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C103" t="s">
-        <v>268</v>
+        <v>380</v>
       </c>
       <c r="D103" t="s">
-        <v>269</v>
+        <v>180</v>
       </c>
       <c r="E103" t="s">
-        <v>273</v>
+        <v>429</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C104" t="s">
-        <v>268</v>
+        <v>380</v>
       </c>
       <c r="D104" t="s">
-        <v>270</v>
+        <v>414</v>
       </c>
       <c r="E104" t="s">
-        <v>274</v>
+        <v>430</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C105" t="s">
-        <v>268</v>
+        <v>165</v>
       </c>
       <c r="D105" t="s">
-        <v>271</v>
+        <v>166</v>
       </c>
       <c r="E105" t="s">
-        <v>275</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C106" t="s">
-        <v>268</v>
+        <v>165</v>
       </c>
       <c r="D106" t="s">
-        <v>272</v>
+        <v>167</v>
       </c>
       <c r="E106" t="s">
-        <v>276</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C107" t="s">
-        <v>277</v>
+        <v>385</v>
       </c>
       <c r="D107" t="s">
-        <v>278</v>
+        <v>416</v>
       </c>
       <c r="E107" t="s">
-        <v>282</v>
+        <v>415</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C108" t="s">
-        <v>277</v>
+        <v>385</v>
       </c>
       <c r="D108" t="s">
-        <v>279</v>
+        <v>417</v>
       </c>
       <c r="E108" t="s">
-        <v>283</v>
+        <v>415</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C109" t="s">
-        <v>277</v>
+        <v>170</v>
       </c>
       <c r="D109" t="s">
-        <v>281</v>
+        <v>171</v>
       </c>
       <c r="E109" t="s">
-        <v>284</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C110" t="s">
-        <v>277</v>
+        <v>170</v>
       </c>
       <c r="D110" t="s">
-        <v>280</v>
+        <v>172</v>
       </c>
       <c r="E110" t="s">
-        <v>285</v>
+        <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B112" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
-        <v>77</v>
-      </c>
-      <c r="D112">
-        <v>91.9</v>
+        <v>352</v>
+      </c>
+      <c r="D112" t="s">
+        <v>353</v>
       </c>
       <c r="E112" t="s">
-        <v>78</v>
+        <v>358</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C113" t="s">
-        <v>77</v>
-      </c>
-      <c r="D113">
-        <v>94.5</v>
+        <v>352</v>
+      </c>
+      <c r="D113" t="s">
+        <v>354</v>
       </c>
       <c r="E113" t="s">
-        <v>79</v>
+        <v>359</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C114" t="s">
-        <v>77</v>
-      </c>
-      <c r="D114">
-        <v>96.1</v>
+        <v>352</v>
+      </c>
+      <c r="D114" t="s">
+        <v>355</v>
       </c>
       <c r="E114" t="s">
-        <v>80</v>
+        <v>360</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B115" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s">
-        <v>77</v>
-      </c>
-      <c r="D115">
-        <v>99.1</v>
+        <v>352</v>
+      </c>
+      <c r="D115" t="s">
+        <v>323</v>
       </c>
       <c r="E115" t="s">
-        <v>81</v>
+        <v>361</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B116" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C116" t="s">
-        <v>95</v>
-      </c>
-      <c r="D116">
-        <v>63</v>
+        <v>352</v>
+      </c>
+      <c r="D116" t="s">
+        <v>356</v>
       </c>
       <c r="E116" t="s">
-        <v>96</v>
+        <v>362</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s">
-        <v>95</v>
-      </c>
-      <c r="D117">
-        <v>150</v>
+        <v>352</v>
+      </c>
+      <c r="D117" t="s">
+        <v>357</v>
       </c>
       <c r="E117" t="s">
-        <v>97</v>
+        <v>363</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C118" t="s">
-        <v>95</v>
-      </c>
-      <c r="D118">
-        <v>330</v>
+        <v>384</v>
+      </c>
+      <c r="D118" t="s">
+        <v>418</v>
       </c>
       <c r="E118" t="s">
-        <v>98</v>
+        <v>415</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
-        <v>95</v>
-      </c>
-      <c r="D119">
-        <v>1000</v>
+        <v>384</v>
+      </c>
+      <c r="D119" t="s">
+        <v>419</v>
       </c>
       <c r="E119" t="s">
-        <v>99</v>
+        <v>415</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B120" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C120" t="s">
-        <v>95</v>
-      </c>
-      <c r="D120">
-        <v>3300</v>
+        <v>175</v>
+      </c>
+      <c r="D120" t="s">
+        <v>176</v>
       </c>
       <c r="E120" t="s">
-        <v>100</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C121" t="s">
-        <v>95</v>
-      </c>
-      <c r="D121">
-        <v>10000</v>
+        <v>175</v>
+      </c>
+      <c r="D121" t="s">
+        <v>177</v>
       </c>
       <c r="E121" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B123" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>95</v>
-      </c>
-      <c r="D123">
-        <v>15000</v>
+        <v>175</v>
+      </c>
+      <c r="D123" t="s">
+        <v>180</v>
       </c>
       <c r="E123" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C124" t="s">
-        <v>95</v>
-      </c>
-      <c r="D124">
-        <v>33000</v>
+        <v>175</v>
+      </c>
+      <c r="D124" t="s">
+        <v>181</v>
       </c>
       <c r="E124" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C125" t="s">
-        <v>82</v>
+        <v>383</v>
       </c>
       <c r="D125" t="s">
-        <v>83</v>
+        <v>420</v>
       </c>
       <c r="E125" t="s">
-        <v>89</v>
+        <v>422</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B126" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C126" t="s">
-        <v>82</v>
+        <v>383</v>
       </c>
       <c r="D126" t="s">
-        <v>84</v>
+        <v>421</v>
       </c>
       <c r="E126" t="s">
-        <v>90</v>
+        <v>423</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B127" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C127" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="D127" t="s">
-        <v>85</v>
+        <v>185</v>
       </c>
       <c r="E127" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B128" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C128" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="D128" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
       <c r="E128" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C129" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="D129" t="s">
-        <v>87</v>
+        <v>187</v>
       </c>
       <c r="E129" t="s">
-        <v>93</v>
+        <v>192</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C130" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="D130" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="E130" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C131" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="D131" t="s">
-        <v>104</v>
+        <v>193</v>
       </c>
       <c r="E131" t="s">
-        <v>106</v>
+        <v>195</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B132" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C132" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="D132" t="s">
-        <v>105</v>
+        <v>194</v>
       </c>
       <c r="E132" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3412,16 +3709,16 @@
         <v>7</v>
       </c>
       <c r="B134" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C134" t="s">
-        <v>286</v>
+        <v>184</v>
       </c>
       <c r="D134" t="s">
-        <v>287</v>
+        <v>197</v>
       </c>
       <c r="E134" t="s">
-        <v>288</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3429,16 +3726,16 @@
         <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C135" t="s">
-        <v>286</v>
+        <v>184</v>
       </c>
       <c r="D135" t="s">
-        <v>289</v>
+        <v>198</v>
       </c>
       <c r="E135" t="s">
-        <v>290</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3446,16 +3743,16 @@
         <v>7</v>
       </c>
       <c r="B136" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C136" t="s">
-        <v>286</v>
+        <v>184</v>
       </c>
       <c r="D136" t="s">
-        <v>291</v>
+        <v>201</v>
       </c>
       <c r="E136" t="s">
-        <v>295</v>
+        <v>203</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3463,16 +3760,16 @@
         <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C137" t="s">
-        <v>286</v>
+        <v>184</v>
       </c>
       <c r="D137" t="s">
-        <v>292</v>
+        <v>202</v>
       </c>
       <c r="E137" t="s">
-        <v>296</v>
+        <v>204</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3480,16 +3777,16 @@
         <v>7</v>
       </c>
       <c r="B138" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C138" t="s">
-        <v>286</v>
+        <v>205</v>
       </c>
       <c r="D138" t="s">
-        <v>293</v>
+        <v>206</v>
       </c>
       <c r="E138" t="s">
-        <v>297</v>
+        <v>208</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3497,16 +3794,16 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C139" t="s">
-        <v>286</v>
+        <v>205</v>
       </c>
       <c r="D139" t="s">
-        <v>294</v>
+        <v>207</v>
       </c>
       <c r="E139" t="s">
-        <v>298</v>
+        <v>209</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3514,16 +3811,16 @@
         <v>7</v>
       </c>
       <c r="B140" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C140" t="s">
-        <v>299</v>
+        <v>210</v>
       </c>
       <c r="D140" t="s">
-        <v>300</v>
+        <v>211</v>
       </c>
       <c r="E140" t="s">
-        <v>302</v>
+        <v>213</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3531,16 +3828,16 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C141" t="s">
-        <v>299</v>
+        <v>210</v>
       </c>
       <c r="D141" t="s">
-        <v>301</v>
+        <v>212</v>
       </c>
       <c r="E141" t="s">
-        <v>303</v>
+        <v>214</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3548,16 +3845,16 @@
         <v>7</v>
       </c>
       <c r="B142" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C142" t="s">
-        <v>304</v>
+        <v>215</v>
       </c>
       <c r="D142" t="s">
-        <v>305</v>
+        <v>193</v>
       </c>
       <c r="E142" t="s">
-        <v>307</v>
+        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3565,16 +3862,16 @@
         <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C143" t="s">
-        <v>304</v>
+        <v>215</v>
       </c>
       <c r="D143" t="s">
-        <v>306</v>
+        <v>216</v>
       </c>
       <c r="E143" t="s">
-        <v>308</v>
+        <v>220</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3582,16 +3879,16 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C145" t="s">
-        <v>309</v>
+        <v>215</v>
       </c>
       <c r="D145" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="E145" t="s">
-        <v>314</v>
+        <v>221</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3599,16 +3896,16 @@
         <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C146" t="s">
-        <v>309</v>
+        <v>215</v>
       </c>
       <c r="D146" t="s">
-        <v>311</v>
+        <v>218</v>
       </c>
       <c r="E146" t="s">
-        <v>315</v>
+        <v>222</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3616,16 +3913,16 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C147" t="s">
-        <v>309</v>
+        <v>223</v>
       </c>
       <c r="D147" t="s">
-        <v>312</v>
+        <v>224</v>
       </c>
       <c r="E147" t="s">
-        <v>316</v>
+        <v>226</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3633,16 +3930,16 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C148" t="s">
-        <v>309</v>
+        <v>223</v>
       </c>
       <c r="D148" t="s">
-        <v>313</v>
+        <v>225</v>
       </c>
       <c r="E148" t="s">
-        <v>317</v>
+        <v>227</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3650,16 +3947,16 @@
         <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C149" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
       <c r="D149" t="s">
-        <v>319</v>
+        <v>229</v>
       </c>
       <c r="E149" t="s">
-        <v>321</v>
+        <v>233</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3667,16 +3964,16 @@
         <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C150" t="s">
-        <v>318</v>
+        <v>228</v>
       </c>
       <c r="D150" t="s">
-        <v>320</v>
+        <v>230</v>
       </c>
       <c r="E150" t="s">
-        <v>322</v>
+        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3684,16 +3981,16 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C151" t="s">
-        <v>323</v>
+        <v>228</v>
       </c>
       <c r="D151" t="s">
-        <v>324</v>
+        <v>231</v>
       </c>
       <c r="E151" t="s">
-        <v>328</v>
+        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,16 +3998,16 @@
         <v>7</v>
       </c>
       <c r="B152" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C152" t="s">
-        <v>323</v>
+        <v>228</v>
       </c>
       <c r="D152" t="s">
-        <v>325</v>
+        <v>232</v>
       </c>
       <c r="E152" t="s">
-        <v>329</v>
+        <v>236</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3718,16 +4015,16 @@
         <v>7</v>
       </c>
       <c r="B153" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C153" t="s">
-        <v>323</v>
+        <v>381</v>
       </c>
       <c r="D153" t="s">
-        <v>326</v>
+        <v>424</v>
       </c>
       <c r="E153" t="s">
-        <v>331</v>
+        <v>426</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3735,16 +4032,764 @@
         <v>7</v>
       </c>
       <c r="B154" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C154" t="s">
-        <v>323</v>
+        <v>381</v>
       </c>
       <c r="D154" t="s">
-        <v>327</v>
+        <v>425</v>
       </c>
       <c r="E154" t="s">
-        <v>330</v>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>8</v>
+      </c>
+      <c r="B156" t="s">
+        <v>108</v>
+      </c>
+      <c r="C156" t="s">
+        <v>237</v>
+      </c>
+      <c r="D156" t="s">
+        <v>238</v>
+      </c>
+      <c r="E156" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>8</v>
+      </c>
+      <c r="B157" t="s">
+        <v>109</v>
+      </c>
+      <c r="C157" t="s">
+        <v>237</v>
+      </c>
+      <c r="D157" t="s">
+        <v>239</v>
+      </c>
+      <c r="E157" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>8</v>
+      </c>
+      <c r="B158" t="s">
+        <v>110</v>
+      </c>
+      <c r="C158" t="s">
+        <v>242</v>
+      </c>
+      <c r="D158" t="s">
+        <v>243</v>
+      </c>
+      <c r="E158" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>8</v>
+      </c>
+      <c r="B159" t="s">
+        <v>111</v>
+      </c>
+      <c r="C159" t="s">
+        <v>242</v>
+      </c>
+      <c r="D159" t="s">
+        <v>244</v>
+      </c>
+      <c r="E159" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>8</v>
+      </c>
+      <c r="B160" t="s">
+        <v>112</v>
+      </c>
+      <c r="C160" t="s">
+        <v>242</v>
+      </c>
+      <c r="D160" t="s">
+        <v>245</v>
+      </c>
+      <c r="E160" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>8</v>
+      </c>
+      <c r="B161" t="s">
+        <v>113</v>
+      </c>
+      <c r="C161" t="s">
+        <v>242</v>
+      </c>
+      <c r="D161" t="s">
+        <v>246</v>
+      </c>
+      <c r="E161" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>8</v>
+      </c>
+      <c r="B162" t="s">
+        <v>114</v>
+      </c>
+      <c r="C162" t="s">
+        <v>251</v>
+      </c>
+      <c r="D162" t="s">
+        <v>252</v>
+      </c>
+      <c r="E162" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>8</v>
+      </c>
+      <c r="B163" t="s">
+        <v>115</v>
+      </c>
+      <c r="C163" t="s">
+        <v>251</v>
+      </c>
+      <c r="D163" t="s">
+        <v>253</v>
+      </c>
+      <c r="E163" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>8</v>
+      </c>
+      <c r="B164" t="s">
+        <v>116</v>
+      </c>
+      <c r="C164" t="s">
+        <v>256</v>
+      </c>
+      <c r="D164" t="s">
+        <v>257</v>
+      </c>
+      <c r="E164" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>8</v>
+      </c>
+      <c r="B165" t="s">
+        <v>117</v>
+      </c>
+      <c r="C165" t="s">
+        <v>256</v>
+      </c>
+      <c r="D165" t="s">
+        <v>258</v>
+      </c>
+      <c r="E165" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>8</v>
+      </c>
+      <c r="B167" t="s">
+        <v>118</v>
+      </c>
+      <c r="C167" t="s">
+        <v>261</v>
+      </c>
+      <c r="D167" t="s">
+        <v>262</v>
+      </c>
+      <c r="E167" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>8</v>
+      </c>
+      <c r="B168" t="s">
+        <v>119</v>
+      </c>
+      <c r="C168" t="s">
+        <v>261</v>
+      </c>
+      <c r="D168" t="s">
+        <v>263</v>
+      </c>
+      <c r="E168" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>8</v>
+      </c>
+      <c r="B169" t="s">
+        <v>120</v>
+      </c>
+      <c r="C169" t="s">
+        <v>364</v>
+      </c>
+      <c r="D169" t="s">
+        <v>322</v>
+      </c>
+      <c r="E169" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>8</v>
+      </c>
+      <c r="B170" t="s">
+        <v>121</v>
+      </c>
+      <c r="C170" t="s">
+        <v>364</v>
+      </c>
+      <c r="D170" t="s">
+        <v>428</v>
+      </c>
+      <c r="E170" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>8</v>
+      </c>
+      <c r="B171" t="s">
+        <v>122</v>
+      </c>
+      <c r="C171" t="s">
+        <v>266</v>
+      </c>
+      <c r="D171" t="s">
+        <v>267</v>
+      </c>
+      <c r="E171" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>8</v>
+      </c>
+      <c r="B172" t="s">
+        <v>123</v>
+      </c>
+      <c r="C172" t="s">
+        <v>266</v>
+      </c>
+      <c r="D172" t="s">
+        <v>268</v>
+      </c>
+      <c r="E172" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>8</v>
+      </c>
+      <c r="B173" t="s">
+        <v>124</v>
+      </c>
+      <c r="C173" t="s">
+        <v>266</v>
+      </c>
+      <c r="D173" t="s">
+        <v>269</v>
+      </c>
+      <c r="E173" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>8</v>
+      </c>
+      <c r="B174" t="s">
+        <v>125</v>
+      </c>
+      <c r="C174" t="s">
+        <v>266</v>
+      </c>
+      <c r="D174" t="s">
+        <v>270</v>
+      </c>
+      <c r="E174" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>8</v>
+      </c>
+      <c r="B175" t="s">
+        <v>126</v>
+      </c>
+      <c r="C175" t="s">
+        <v>275</v>
+      </c>
+      <c r="D175" t="s">
+        <v>276</v>
+      </c>
+      <c r="E175" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>8</v>
+      </c>
+      <c r="B176" t="s">
+        <v>127</v>
+      </c>
+      <c r="C176" t="s">
+        <v>275</v>
+      </c>
+      <c r="D176" t="s">
+        <v>277</v>
+      </c>
+      <c r="E176" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>9</v>
+      </c>
+      <c r="B178" t="s">
+        <v>108</v>
+      </c>
+      <c r="C178" t="s">
+        <v>275</v>
+      </c>
+      <c r="D178" t="s">
+        <v>279</v>
+      </c>
+      <c r="E178" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>9</v>
+      </c>
+      <c r="B179" t="s">
+        <v>109</v>
+      </c>
+      <c r="C179" t="s">
+        <v>275</v>
+      </c>
+      <c r="D179" t="s">
+        <v>278</v>
+      </c>
+      <c r="E179" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>9</v>
+      </c>
+      <c r="B180" t="s">
+        <v>110</v>
+      </c>
+      <c r="C180" t="s">
+        <v>284</v>
+      </c>
+      <c r="D180" t="s">
+        <v>285</v>
+      </c>
+      <c r="E180" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>9</v>
+      </c>
+      <c r="B181" t="s">
+        <v>111</v>
+      </c>
+      <c r="C181" t="s">
+        <v>284</v>
+      </c>
+      <c r="D181" t="s">
+        <v>287</v>
+      </c>
+      <c r="E181" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>9</v>
+      </c>
+      <c r="B182" t="s">
+        <v>112</v>
+      </c>
+      <c r="C182" t="s">
+        <v>284</v>
+      </c>
+      <c r="D182" t="s">
+        <v>289</v>
+      </c>
+      <c r="E182" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>9</v>
+      </c>
+      <c r="B183" t="s">
+        <v>113</v>
+      </c>
+      <c r="C183" t="s">
+        <v>284</v>
+      </c>
+      <c r="D183" t="s">
+        <v>290</v>
+      </c>
+      <c r="E183" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>9</v>
+      </c>
+      <c r="B184" t="s">
+        <v>114</v>
+      </c>
+      <c r="C184" t="s">
+        <v>284</v>
+      </c>
+      <c r="D184" t="s">
+        <v>291</v>
+      </c>
+      <c r="E184" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>9</v>
+      </c>
+      <c r="B185" t="s">
+        <v>115</v>
+      </c>
+      <c r="C185" t="s">
+        <v>284</v>
+      </c>
+      <c r="D185" t="s">
+        <v>292</v>
+      </c>
+      <c r="E185" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>9</v>
+      </c>
+      <c r="B186" t="s">
+        <v>116</v>
+      </c>
+      <c r="C186" t="s">
+        <v>365</v>
+      </c>
+      <c r="D186" t="s">
+        <v>366</v>
+      </c>
+      <c r="E186" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>9</v>
+      </c>
+      <c r="B187" t="s">
+        <v>117</v>
+      </c>
+      <c r="C187" t="s">
+        <v>365</v>
+      </c>
+      <c r="D187" t="s">
+        <v>367</v>
+      </c>
+      <c r="E187" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>10</v>
+      </c>
+      <c r="B189" t="s">
+        <v>118</v>
+      </c>
+      <c r="C189" t="s">
+        <v>297</v>
+      </c>
+      <c r="D189" t="s">
+        <v>298</v>
+      </c>
+      <c r="E189" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>10</v>
+      </c>
+      <c r="B190" t="s">
+        <v>119</v>
+      </c>
+      <c r="C190" t="s">
+        <v>297</v>
+      </c>
+      <c r="D190" t="s">
+        <v>299</v>
+      </c>
+      <c r="E190" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>10</v>
+      </c>
+      <c r="B191" t="s">
+        <v>120</v>
+      </c>
+      <c r="C191" t="s">
+        <v>302</v>
+      </c>
+      <c r="D191" t="s">
+        <v>303</v>
+      </c>
+      <c r="E191" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>10</v>
+      </c>
+      <c r="B192" t="s">
+        <v>121</v>
+      </c>
+      <c r="C192" t="s">
+        <v>302</v>
+      </c>
+      <c r="D192" t="s">
+        <v>304</v>
+      </c>
+      <c r="E192" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>10</v>
+      </c>
+      <c r="B193" t="s">
+        <v>122</v>
+      </c>
+      <c r="C193" t="s">
+        <v>307</v>
+      </c>
+      <c r="D193" t="s">
+        <v>308</v>
+      </c>
+      <c r="E193" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>10</v>
+      </c>
+      <c r="B194" t="s">
+        <v>123</v>
+      </c>
+      <c r="C194" t="s">
+        <v>307</v>
+      </c>
+      <c r="D194" t="s">
+        <v>309</v>
+      </c>
+      <c r="E194" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>10</v>
+      </c>
+      <c r="B195" t="s">
+        <v>124</v>
+      </c>
+      <c r="C195" t="s">
+        <v>307</v>
+      </c>
+      <c r="D195" t="s">
+        <v>310</v>
+      </c>
+      <c r="E195" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>10</v>
+      </c>
+      <c r="B196" t="s">
+        <v>125</v>
+      </c>
+      <c r="C196" t="s">
+        <v>307</v>
+      </c>
+      <c r="D196" t="s">
+        <v>311</v>
+      </c>
+      <c r="E196" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>10</v>
+      </c>
+      <c r="B197" t="s">
+        <v>126</v>
+      </c>
+      <c r="C197" t="s">
+        <v>316</v>
+      </c>
+      <c r="D197" t="s">
+        <v>317</v>
+      </c>
+      <c r="E197" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>10</v>
+      </c>
+      <c r="B198" t="s">
+        <v>127</v>
+      </c>
+      <c r="C198" t="s">
+        <v>316</v>
+      </c>
+      <c r="D198" t="s">
+        <v>318</v>
+      </c>
+      <c r="E198" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>10</v>
+      </c>
+      <c r="B200" t="s">
+        <v>108</v>
+      </c>
+      <c r="C200" t="s">
+        <v>370</v>
+      </c>
+      <c r="D200" t="s">
+        <v>371</v>
+      </c>
+      <c r="E200" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>10</v>
+      </c>
+      <c r="B201" t="s">
+        <v>109</v>
+      </c>
+      <c r="C201" t="s">
+        <v>370</v>
+      </c>
+      <c r="D201" t="s">
+        <v>372</v>
+      </c>
+      <c r="E201" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>10</v>
+      </c>
+      <c r="B202" t="s">
+        <v>110</v>
+      </c>
+      <c r="C202" t="s">
+        <v>370</v>
+      </c>
+      <c r="D202" t="s">
+        <v>373</v>
+      </c>
+      <c r="E202" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>10</v>
+      </c>
+      <c r="B203" t="s">
+        <v>111</v>
+      </c>
+      <c r="C203" t="s">
+        <v>370</v>
+      </c>
+      <c r="D203" t="s">
+        <v>374</v>
+      </c>
+      <c r="E203" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated titles yet again
</commit_message>
<xml_diff>
--- a/titles/songs.xlsx
+++ b/titles/songs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\pi\pi-seeburg\titles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="songs" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="440">
   <si>
     <t>Artist</t>
   </si>
@@ -260,18 +260,6 @@
     <t>Radio</t>
   </si>
   <si>
-    <t>radio:91.9</t>
-  </si>
-  <si>
-    <t>radio:94.5</t>
-  </si>
-  <si>
-    <t>radio:96.1</t>
-  </si>
-  <si>
-    <t>radio:99.1</t>
-  </si>
-  <si>
     <t>Kevin MacLeod</t>
   </si>
   <si>
@@ -1202,9 +1190,6 @@
     <t>/music/ABC/BestOf/03. Poison Arrow.wav</t>
   </si>
   <si>
-    <t>King Without A Crow</t>
-  </si>
-  <si>
     <t>/music/ABC/BestOf/12. King Without a Crown.wav</t>
   </si>
   <si>
@@ -1253,76 +1238,118 @@
     <t>Conga</t>
   </si>
   <si>
+    <t>/music/Gloria Estefan/TheEssentialCD1/02 Rhythm Is Gonna Get You.wav</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD1/04 Everlasting Love (Video Version).wav</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD1/18 Conga.wav</t>
+  </si>
+  <si>
+    <t>/music/Gloria Estefan/TheEssentialCD2/15 - Gloria Estefan - Hold Me, Thrill Me, Kiss Me.wav</t>
+  </si>
+  <si>
+    <t>Ring of Ice</t>
+  </si>
+  <si>
+    <t>Is This a Cool World or What</t>
+  </si>
+  <si>
+    <t>Midnight Confessions</t>
+  </si>
+  <si>
+    <t>Free World</t>
+  </si>
+  <si>
+    <t>In These Shoes</t>
+  </si>
+  <si>
+    <t>Kiss Me Deadly</t>
+  </si>
+  <si>
+    <t>Under The Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/music/Lita Ford/Greatest/04-Kiss Me Deadly.wav </t>
+  </si>
+  <si>
+    <t>/music/Lita Ford/Greatest/07-Under The Gun.wav</t>
+  </si>
+  <si>
+    <t>Harden My Heart</t>
+  </si>
+  <si>
+    <t>Find Another Fool</t>
+  </si>
+  <si>
+    <t>/music/Quarterflash/GreatestHits/01. Harden My Heart - Quarterflash.wav</t>
+  </si>
+  <si>
+    <t>/music/Quarterflash/GreatestHits/02. Find Another Fool - Quarterflash.wav</t>
+  </si>
+  <si>
+    <t>/music/Jennifer Rush/TheVeryBestOf1/[01] [Jennifer Rush] The Power Of Love (Special Edit Version - Previously Unreleased).wav</t>
+  </si>
+  <si>
+    <t>/music/Jennifer Rush/TheVeryBestOf1/[03] [Jennifer Rush] Ring Of Ice (Special Edit Version).wav</t>
+  </si>
+  <si>
     <t>Hold Me, Thrill Me, Kiss Me</t>
   </si>
   <si>
-    <t>/music/Gloria Estefan/TheEssentialCD1/02 Rhythm Is Gonna Get You.wav</t>
-  </si>
-  <si>
-    <t>/music/Gloria Estefan/TheEssentialCD1/04 Everlasting Love (Video Version).wav</t>
-  </si>
-  <si>
-    <t>/music/Gloria Estefan/TheEssentialCD1/18 Conga.wav</t>
-  </si>
-  <si>
-    <t>/music/Gloria Estefan/TheEssentialCD2/15 - Gloria Estefan - Hold Me, Thrill Me, Kiss Me.wav</t>
-  </si>
-  <si>
-    <t>Ring of Ice</t>
-  </si>
-  <si>
-    <t>nofn</t>
-  </si>
-  <si>
-    <t>Is This a Cool World or What</t>
-  </si>
-  <si>
-    <t>Midnight Confessions</t>
-  </si>
-  <si>
-    <t>Free World</t>
-  </si>
-  <si>
-    <t>In These Shoes</t>
-  </si>
-  <si>
-    <t>Kiss Me Deadly</t>
-  </si>
-  <si>
-    <t>Under The Gun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/music/Lita Ford/Greatest/04-Kiss Me Deadly.wav </t>
-  </si>
-  <si>
-    <t>/music/Lita Ford/Greatest/07-Under The Gun.wav</t>
-  </si>
-  <si>
-    <t>Harden My Heart</t>
-  </si>
-  <si>
-    <t>Find Another Fool</t>
-  </si>
-  <si>
-    <t>/music/Quarterflash/GreatestHits/01. Harden My Heart - Quarterflash.wav</t>
-  </si>
-  <si>
-    <t>/music/Quarterflash/GreatestHits/02. Find Another Fool - Quarterflash.wav</t>
-  </si>
-  <si>
-    <t>Better Than Heaver</t>
-  </si>
-  <si>
-    <t>/music/Jennifer Rush/TheVeryBestOf1/[01] [Jennifer Rush] The Power Of Love (Special Edit Version - Previously Unreleased).wav</t>
-  </si>
-  <si>
-    <t>/music/Jennifer Rush/TheVeryBestOf1/[03] [Jennifer Rush] Ring Of Ice (Special Edit Version).wav</t>
+    <t>King Without A Crown</t>
+  </si>
+  <si>
+    <t>Better Than Heaven</t>
+  </si>
+  <si>
+    <t>Love Shack</t>
+  </si>
+  <si>
+    <t>52 Girls</t>
+  </si>
+  <si>
+    <t>radio:919</t>
+  </si>
+  <si>
+    <t>radio:945</t>
+  </si>
+  <si>
+    <t>radio:961</t>
+  </si>
+  <si>
+    <t>radio:991</t>
+  </si>
+  <si>
+    <t>/music/Karla Devito/Is This A Cool World Or What 1981/01 Is This a Cool World or What.wav</t>
+  </si>
+  <si>
+    <t>/music/Karla Devito/Is This A Cool World Or What 1981/04 Midnight Confessions.wav</t>
+  </si>
+  <si>
+    <t>/music/Stacey Q/Greatest/01. Two of Hearts - Stacey Q.wav</t>
+  </si>
+  <si>
+    <t>/music/Kirsty MacColl/TropicalBrainstorm/Track02.wav</t>
+  </si>
+  <si>
+    <t>/music/Kirsty MacColl/Kite/02 - Free World.wav</t>
+  </si>
+  <si>
+    <t>/music/Stacey Q/BetterThanHeaven/04 - Better Than Heaven.wav</t>
+  </si>
+  <si>
+    <t>/music/The B-52's/TimeCapsule/13 Love Shack.wav</t>
+  </si>
+  <si>
+    <t>/music/The B-52's/TimeCapsule/02 52 Girls.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1633,11 +1660,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E203"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,10 +1676,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1669,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -1678,7 +1705,7 @@
         <v>91.9</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1686,7 +1713,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -1695,7 +1722,7 @@
         <v>94.5</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1703,7 +1730,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>77</v>
@@ -1712,7 +1739,7 @@
         <v>96.1</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,7 +1747,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>77</v>
@@ -1729,7 +1756,7 @@
         <v>99.1</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,16 +1764,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" t="s">
         <v>324</v>
       </c>
-      <c r="D6" t="s">
-        <v>328</v>
-      </c>
       <c r="E6" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1754,16 +1781,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1771,16 +1798,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D8">
         <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1788,16 +1815,16 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D9">
         <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1805,16 +1832,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D10">
         <v>330</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1822,16 +1849,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D11">
         <v>1000</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1839,16 +1866,16 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D13">
         <v>3300</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,16 +1883,16 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D14">
         <v>10000</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1873,16 +1900,16 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1890,16 +1917,16 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1907,16 +1934,16 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,16 +1951,16 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
         <v>82</v>
       </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1941,16 +1968,16 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,16 +1985,16 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1975,16 +2002,16 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1992,16 +2019,16 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,16 +2036,16 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C24" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D24" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E24" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2026,16 +2053,16 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
+        <v>338</v>
+      </c>
+      <c r="D25" t="s">
+        <v>340</v>
+      </c>
+      <c r="E25" t="s">
         <v>342</v>
-      </c>
-      <c r="D25" t="s">
-        <v>344</v>
-      </c>
-      <c r="E25" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2043,16 +2070,16 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D26" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E26" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2060,16 +2087,16 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D27" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E27" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2077,16 +2104,16 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D28" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E28" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2094,16 +2121,16 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
+        <v>333</v>
+      </c>
+      <c r="D29" t="s">
+        <v>335</v>
+      </c>
+      <c r="E29" t="s">
         <v>337</v>
-      </c>
-      <c r="D29" t="s">
-        <v>339</v>
-      </c>
-      <c r="E29" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2111,16 +2138,16 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D30" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E30" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2128,16 +2155,16 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D31" t="s">
-        <v>392</v>
+        <v>424</v>
       </c>
       <c r="E31" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2145,7 +2172,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
         <v>24</v>
@@ -2162,7 +2189,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
         <v>24</v>
@@ -2179,16 +2206,16 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E35" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2196,16 +2223,16 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
         <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E36" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2213,16 +2240,16 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
+        <v>325</v>
+      </c>
+      <c r="D37" t="s">
+        <v>317</v>
+      </c>
+      <c r="E37" t="s">
         <v>329</v>
-      </c>
-      <c r="D37" t="s">
-        <v>321</v>
-      </c>
-      <c r="E37" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2230,16 +2257,16 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D38" t="s">
+        <v>326</v>
+      </c>
+      <c r="E38" t="s">
         <v>330</v>
-      </c>
-      <c r="E38" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2247,16 +2274,16 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D39" t="s">
+        <v>327</v>
+      </c>
+      <c r="E39" t="s">
         <v>331</v>
-      </c>
-      <c r="E39" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2264,16 +2291,16 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D40" t="s">
+        <v>328</v>
+      </c>
+      <c r="E40" t="s">
         <v>332</v>
-      </c>
-      <c r="E40" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2281,7 +2308,7 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
@@ -2298,7 +2325,7 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
         <v>29</v>
@@ -2315,16 +2342,16 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
         <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E43" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2332,16 +2359,16 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
         <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="E44" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2349,7 +2376,7 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -2366,7 +2393,7 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -2383,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -2400,7 +2427,7 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -2417,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -2434,7 +2461,7 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -2451,7 +2478,7 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -2468,7 +2495,7 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -2485,7 +2512,7 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -2502,7 +2529,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -2519,7 +2546,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
         <v>34</v>
@@ -2536,7 +2563,7 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C58" t="s">
         <v>34</v>
@@ -2553,7 +2580,7 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
         <v>39</v>
@@ -2570,7 +2597,7 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
         <v>39</v>
@@ -2587,7 +2614,7 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
         <v>45</v>
@@ -2604,7 +2631,7 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C62" t="s">
         <v>45</v>
@@ -2621,7 +2648,7 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C63" t="s">
         <v>49</v>
@@ -2638,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C64" t="s">
         <v>49</v>
@@ -2655,7 +2682,7 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
         <v>49</v>
@@ -2672,7 +2699,7 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
         <v>49</v>
@@ -2689,7 +2716,7 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C68" t="s">
         <v>49</v>
@@ -2706,7 +2733,7 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C69" t="s">
         <v>49</v>
@@ -2723,16 +2750,16 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D70" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E70" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2740,16 +2767,16 @@
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
+        <v>343</v>
+      </c>
+      <c r="D71" t="s">
+        <v>345</v>
+      </c>
+      <c r="E71" t="s">
         <v>347</v>
-      </c>
-      <c r="D71" t="s">
-        <v>349</v>
-      </c>
-      <c r="E71" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2757,7 +2784,7 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C72" t="s">
         <v>62</v>
@@ -2774,7 +2801,7 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C73" t="s">
         <v>62</v>
@@ -2791,7 +2818,7 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C74" t="s">
         <v>67</v>
@@ -2808,7 +2835,7 @@
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C75" t="s">
         <v>67</v>
@@ -2825,7 +2852,7 @@
         <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
         <v>72</v>
@@ -2842,7 +2869,7 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C77" t="s">
         <v>72</v>
@@ -2859,16 +2886,16 @@
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C79" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D79" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E79" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,16 +2903,16 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C80" t="s">
+        <v>124</v>
+      </c>
+      <c r="D80" t="s">
+        <v>126</v>
+      </c>
+      <c r="E80" t="s">
         <v>128</v>
-      </c>
-      <c r="D80" t="s">
-        <v>130</v>
-      </c>
-      <c r="E80" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2893,16 +2920,16 @@
         <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C81" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D81" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E81" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2910,16 +2937,16 @@
         <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D82" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E82" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2927,16 +2954,16 @@
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" t="s">
         <v>133</v>
       </c>
-      <c r="D83" t="s">
-        <v>137</v>
-      </c>
       <c r="E83" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2944,16 +2971,16 @@
         <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E84" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2961,16 +2988,16 @@
         <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C85" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D85" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E85" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2978,16 +3005,16 @@
         <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C86" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D86" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E86" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2995,16 +3022,16 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C87" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E87" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,16 +3039,16 @@
         <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C88" t="s">
+        <v>138</v>
+      </c>
+      <c r="D88" t="s">
+        <v>140</v>
+      </c>
+      <c r="E88" t="s">
         <v>142</v>
-      </c>
-      <c r="D88" t="s">
-        <v>144</v>
-      </c>
-      <c r="E88" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,16 +3056,16 @@
         <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C90" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D90" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="E90" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3046,16 +3073,16 @@
         <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C91" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D91" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="E91" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3063,16 +3090,16 @@
         <v>2</v>
       </c>
       <c r="B92" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C92" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D92" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E92" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3080,16 +3107,16 @@
         <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C93" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D93" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="E93" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,16 +3124,16 @@
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C94" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D94" t="s">
+        <v>144</v>
+      </c>
+      <c r="E94" t="s">
         <v>148</v>
-      </c>
-      <c r="E94" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,16 +3141,16 @@
         <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C95" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D95" t="s">
+        <v>145</v>
+      </c>
+      <c r="E95" t="s">
         <v>149</v>
-      </c>
-      <c r="E95" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3158,16 @@
         <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C96" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D96" t="s">
+        <v>146</v>
+      </c>
+      <c r="E96" t="s">
         <v>150</v>
-      </c>
-      <c r="E96" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,16 +3175,16 @@
         <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C97" t="s">
+        <v>143</v>
+      </c>
+      <c r="D97" t="s">
         <v>147</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>151</v>
-      </c>
-      <c r="E97" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3165,16 +3192,16 @@
         <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C98" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D98" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E98" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,16 +3209,16 @@
         <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C99" t="s">
+        <v>152</v>
+      </c>
+      <c r="D99" t="s">
+        <v>154</v>
+      </c>
+      <c r="E99" t="s">
         <v>156</v>
-      </c>
-      <c r="D99" t="s">
-        <v>158</v>
-      </c>
-      <c r="E99" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,16 +3226,16 @@
         <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C101" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D101" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E101" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,16 +3243,16 @@
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C102" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D102" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E102" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3233,16 +3260,16 @@
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C103" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D103" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E103" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3250,16 +3277,16 @@
         <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C104" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D104" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="E104" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3267,16 +3294,16 @@
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D105" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E105" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3284,16 +3311,16 @@
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C106" t="s">
+        <v>161</v>
+      </c>
+      <c r="D106" t="s">
+        <v>163</v>
+      </c>
+      <c r="E106" t="s">
         <v>165</v>
-      </c>
-      <c r="D106" t="s">
-        <v>167</v>
-      </c>
-      <c r="E106" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3328,16 @@
         <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C107" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D107" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="E107" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3318,16 +3345,16 @@
         <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C108" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D108" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="E108" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3335,16 +3362,16 @@
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C109" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D109" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E109" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3379,16 @@
         <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C110" t="s">
+        <v>166</v>
+      </c>
+      <c r="D110" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" t="s">
         <v>170</v>
-      </c>
-      <c r="D110" t="s">
-        <v>172</v>
-      </c>
-      <c r="E110" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3369,16 +3396,16 @@
         <v>1</v>
       </c>
       <c r="B112" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C112" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D112" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E112" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3386,16 +3413,16 @@
         <v>1</v>
       </c>
       <c r="B113" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C113" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D113" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E113" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3403,16 +3430,16 @@
         <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C114" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D114" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E114" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,16 +3447,16 @@
         <v>1</v>
       </c>
       <c r="B115" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C115" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D115" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E115" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3437,16 +3464,16 @@
         <v>1</v>
       </c>
       <c r="B116" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C116" t="s">
+        <v>348</v>
+      </c>
+      <c r="D116" t="s">
         <v>352</v>
       </c>
-      <c r="D116" t="s">
-        <v>356</v>
-      </c>
       <c r="E116" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3454,16 +3481,16 @@
         <v>1</v>
       </c>
       <c r="B117" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C117" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D117" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E117" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3471,16 +3498,16 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C118" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D118" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="E118" t="s">
-        <v>415</v>
+        <v>436</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3488,16 +3515,16 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C119" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D119" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="E119" t="s">
-        <v>415</v>
+        <v>435</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3505,16 +3532,16 @@
         <v>1</v>
       </c>
       <c r="B120" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C120" t="s">
+        <v>171</v>
+      </c>
+      <c r="D120" t="s">
+        <v>172</v>
+      </c>
+      <c r="E120" t="s">
         <v>175</v>
-      </c>
-      <c r="D120" t="s">
-        <v>176</v>
-      </c>
-      <c r="E120" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3522,16 +3549,16 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C121" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D121" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E121" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3539,16 +3566,16 @@
         <v>1</v>
       </c>
       <c r="B123" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C123" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D123" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E123" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3556,16 +3583,16 @@
         <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C124" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D124" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E124" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3573,16 +3600,16 @@
         <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C125" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D125" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="E125" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3590,16 +3617,16 @@
         <v>1</v>
       </c>
       <c r="B126" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C126" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D126" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="E126" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3607,16 +3634,16 @@
         <v>1</v>
       </c>
       <c r="B127" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C127" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D127" t="s">
+        <v>181</v>
+      </c>
+      <c r="E127" t="s">
         <v>185</v>
-      </c>
-      <c r="E127" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3624,16 +3651,16 @@
         <v>1</v>
       </c>
       <c r="B128" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C128" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D128" t="s">
+        <v>182</v>
+      </c>
+      <c r="E128" t="s">
         <v>186</v>
-      </c>
-      <c r="E128" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3641,16 +3668,16 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C129" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D129" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E129" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3658,16 +3685,16 @@
         <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C130" t="s">
+        <v>180</v>
+      </c>
+      <c r="D130" t="s">
         <v>184</v>
       </c>
-      <c r="D130" t="s">
-        <v>188</v>
-      </c>
       <c r="E130" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3675,16 +3702,16 @@
         <v>1</v>
       </c>
       <c r="B131" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C131" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D131" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E131" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,16 +3719,16 @@
         <v>1</v>
       </c>
       <c r="B132" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C132" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D132" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E132" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3709,16 +3736,16 @@
         <v>7</v>
       </c>
       <c r="B134" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C134" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D134" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E134" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3726,16 +3753,16 @@
         <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C135" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D135" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E135" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,16 +3770,16 @@
         <v>7</v>
       </c>
       <c r="B136" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C136" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D136" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E136" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3760,16 +3787,16 @@
         <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C137" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D137" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E137" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3777,16 +3804,16 @@
         <v>7</v>
       </c>
       <c r="B138" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C138" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D138" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E138" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,16 +3821,16 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C139" t="s">
+        <v>201</v>
+      </c>
+      <c r="D139" t="s">
+        <v>203</v>
+      </c>
+      <c r="E139" t="s">
         <v>205</v>
-      </c>
-      <c r="D139" t="s">
-        <v>207</v>
-      </c>
-      <c r="E139" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,16 +3838,16 @@
         <v>7</v>
       </c>
       <c r="B140" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C140" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D140" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E140" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,16 +3855,16 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C141" t="s">
+        <v>206</v>
+      </c>
+      <c r="D141" t="s">
+        <v>208</v>
+      </c>
+      <c r="E141" t="s">
         <v>210</v>
-      </c>
-      <c r="D141" t="s">
-        <v>212</v>
-      </c>
-      <c r="E141" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,16 +3872,16 @@
         <v>7</v>
       </c>
       <c r="B142" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C142" t="s">
+        <v>211</v>
+      </c>
+      <c r="D142" t="s">
+        <v>189</v>
+      </c>
+      <c r="E142" t="s">
         <v>215</v>
-      </c>
-      <c r="D142" t="s">
-        <v>193</v>
-      </c>
-      <c r="E142" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,16 +3889,16 @@
         <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C143" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D143" t="s">
+        <v>212</v>
+      </c>
+      <c r="E143" t="s">
         <v>216</v>
-      </c>
-      <c r="E143" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,16 +3906,16 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C145" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D145" t="s">
+        <v>213</v>
+      </c>
+      <c r="E145" t="s">
         <v>217</v>
-      </c>
-      <c r="E145" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3896,16 +3923,16 @@
         <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C146" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D146" t="s">
+        <v>214</v>
+      </c>
+      <c r="E146" t="s">
         <v>218</v>
-      </c>
-      <c r="E146" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,16 +3940,16 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C147" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D147" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E147" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,16 +3957,16 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C148" t="s">
+        <v>219</v>
+      </c>
+      <c r="D148" t="s">
+        <v>221</v>
+      </c>
+      <c r="E148" t="s">
         <v>223</v>
-      </c>
-      <c r="D148" t="s">
-        <v>225</v>
-      </c>
-      <c r="E148" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3947,16 +3974,16 @@
         <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C149" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D149" t="s">
+        <v>225</v>
+      </c>
+      <c r="E149" t="s">
         <v>229</v>
-      </c>
-      <c r="E149" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,16 +3991,16 @@
         <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C150" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D150" t="s">
+        <v>226</v>
+      </c>
+      <c r="E150" t="s">
         <v>230</v>
-      </c>
-      <c r="E150" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3981,16 +4008,16 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C151" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D151" t="s">
+        <v>227</v>
+      </c>
+      <c r="E151" t="s">
         <v>231</v>
-      </c>
-      <c r="E151" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3998,16 +4025,16 @@
         <v>7</v>
       </c>
       <c r="B152" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C152" t="s">
+        <v>224</v>
+      </c>
+      <c r="D152" t="s">
         <v>228</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>232</v>
-      </c>
-      <c r="E152" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4015,16 +4042,16 @@
         <v>7</v>
       </c>
       <c r="B153" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C153" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D153" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E153" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4032,16 +4059,16 @@
         <v>7</v>
       </c>
       <c r="B154" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C154" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D154" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="E154" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4049,16 +4076,16 @@
         <v>8</v>
       </c>
       <c r="B156" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C156" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D156" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E156" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4066,16 +4093,16 @@
         <v>8</v>
       </c>
       <c r="B157" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C157" t="s">
+        <v>233</v>
+      </c>
+      <c r="D157" t="s">
+        <v>235</v>
+      </c>
+      <c r="E157" t="s">
         <v>237</v>
-      </c>
-      <c r="D157" t="s">
-        <v>239</v>
-      </c>
-      <c r="E157" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4083,16 +4110,16 @@
         <v>8</v>
       </c>
       <c r="B158" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C158" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D158" t="s">
+        <v>239</v>
+      </c>
+      <c r="E158" t="s">
         <v>243</v>
-      </c>
-      <c r="E158" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4100,16 +4127,16 @@
         <v>8</v>
       </c>
       <c r="B159" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C159" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D159" t="s">
+        <v>240</v>
+      </c>
+      <c r="E159" t="s">
         <v>244</v>
-      </c>
-      <c r="E159" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4117,16 +4144,16 @@
         <v>8</v>
       </c>
       <c r="B160" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C160" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D160" t="s">
+        <v>241</v>
+      </c>
+      <c r="E160" t="s">
         <v>245</v>
-      </c>
-      <c r="E160" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4134,16 +4161,16 @@
         <v>8</v>
       </c>
       <c r="B161" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C161" t="s">
+        <v>238</v>
+      </c>
+      <c r="D161" t="s">
         <v>242</v>
       </c>
-      <c r="D161" t="s">
+      <c r="E161" t="s">
         <v>246</v>
-      </c>
-      <c r="E161" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4151,16 +4178,16 @@
         <v>8</v>
       </c>
       <c r="B162" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C162" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D162" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E162" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4168,16 +4195,16 @@
         <v>8</v>
       </c>
       <c r="B163" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C163" t="s">
+        <v>247</v>
+      </c>
+      <c r="D163" t="s">
+        <v>249</v>
+      </c>
+      <c r="E163" t="s">
         <v>251</v>
-      </c>
-      <c r="D163" t="s">
-        <v>253</v>
-      </c>
-      <c r="E163" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4185,16 +4212,16 @@
         <v>8</v>
       </c>
       <c r="B164" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C164" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D164" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E164" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4202,16 +4229,16 @@
         <v>8</v>
       </c>
       <c r="B165" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C165" t="s">
+        <v>252</v>
+      </c>
+      <c r="D165" t="s">
+        <v>254</v>
+      </c>
+      <c r="E165" t="s">
         <v>256</v>
-      </c>
-      <c r="D165" t="s">
-        <v>258</v>
-      </c>
-      <c r="E165" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4219,16 +4246,16 @@
         <v>8</v>
       </c>
       <c r="B167" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C167" t="s">
+        <v>257</v>
+      </c>
+      <c r="D167" t="s">
+        <v>258</v>
+      </c>
+      <c r="E167" t="s">
         <v>261</v>
-      </c>
-      <c r="D167" t="s">
-        <v>262</v>
-      </c>
-      <c r="E167" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4236,16 +4263,16 @@
         <v>8</v>
       </c>
       <c r="B168" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C168" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D168" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E168" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4253,16 +4280,16 @@
         <v>8</v>
       </c>
       <c r="B169" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C169" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D169" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E169" t="s">
-        <v>415</v>
+        <v>434</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4270,16 +4297,16 @@
         <v>8</v>
       </c>
       <c r="B170" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C170" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D170" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="E170" t="s">
-        <v>415</v>
+        <v>437</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4287,16 +4314,16 @@
         <v>8</v>
       </c>
       <c r="B171" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C171" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D171" t="s">
+        <v>263</v>
+      </c>
+      <c r="E171" t="s">
         <v>267</v>
-      </c>
-      <c r="E171" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4304,16 +4331,16 @@
         <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C172" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D172" t="s">
+        <v>264</v>
+      </c>
+      <c r="E172" t="s">
         <v>268</v>
-      </c>
-      <c r="E172" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,16 +4348,16 @@
         <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C173" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D173" t="s">
+        <v>265</v>
+      </c>
+      <c r="E173" t="s">
         <v>269</v>
-      </c>
-      <c r="E173" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4338,16 +4365,16 @@
         <v>8</v>
       </c>
       <c r="B174" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C174" t="s">
+        <v>262</v>
+      </c>
+      <c r="D174" t="s">
         <v>266</v>
       </c>
-      <c r="D174" t="s">
+      <c r="E174" t="s">
         <v>270</v>
-      </c>
-      <c r="E174" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4355,16 +4382,16 @@
         <v>8</v>
       </c>
       <c r="B175" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C175" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D175" t="s">
+        <v>272</v>
+      </c>
+      <c r="E175" t="s">
         <v>276</v>
-      </c>
-      <c r="E175" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4372,16 +4399,16 @@
         <v>8</v>
       </c>
       <c r="B176" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C176" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D176" t="s">
+        <v>273</v>
+      </c>
+      <c r="E176" t="s">
         <v>277</v>
-      </c>
-      <c r="E176" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4389,16 +4416,16 @@
         <v>9</v>
       </c>
       <c r="B178" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C178" t="s">
+        <v>271</v>
+      </c>
+      <c r="D178" t="s">
         <v>275</v>
       </c>
-      <c r="D178" t="s">
-        <v>279</v>
-      </c>
       <c r="E178" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4406,16 +4433,16 @@
         <v>9</v>
       </c>
       <c r="B179" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C179" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D179" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E179" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4423,16 +4450,16 @@
         <v>9</v>
       </c>
       <c r="B180" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C180" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D180" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E180" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4440,16 +4467,16 @@
         <v>9</v>
       </c>
       <c r="B181" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C181" t="s">
+        <v>280</v>
+      </c>
+      <c r="D181" t="s">
+        <v>283</v>
+      </c>
+      <c r="E181" t="s">
         <v>284</v>
-      </c>
-      <c r="D181" t="s">
-        <v>287</v>
-      </c>
-      <c r="E181" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4457,16 +4484,16 @@
         <v>9</v>
       </c>
       <c r="B182" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C182" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D182" t="s">
+        <v>285</v>
+      </c>
+      <c r="E182" t="s">
         <v>289</v>
-      </c>
-      <c r="E182" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -4474,16 +4501,16 @@
         <v>9</v>
       </c>
       <c r="B183" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C183" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D183" t="s">
+        <v>286</v>
+      </c>
+      <c r="E183" t="s">
         <v>290</v>
-      </c>
-      <c r="E183" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -4491,16 +4518,16 @@
         <v>9</v>
       </c>
       <c r="B184" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C184" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D184" t="s">
+        <v>287</v>
+      </c>
+      <c r="E184" t="s">
         <v>291</v>
-      </c>
-      <c r="E184" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4508,16 +4535,16 @@
         <v>9</v>
       </c>
       <c r="B185" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C185" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D185" t="s">
+        <v>288</v>
+      </c>
+      <c r="E185" t="s">
         <v>292</v>
-      </c>
-      <c r="E185" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4525,16 +4552,16 @@
         <v>9</v>
       </c>
       <c r="B186" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C186" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D186" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E186" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4542,186 +4569,186 @@
         <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C187" t="s">
+        <v>361</v>
+      </c>
+      <c r="D187" t="s">
+        <v>363</v>
+      </c>
+      <c r="E187" t="s">
         <v>365</v>
-      </c>
-      <c r="D187" t="s">
-        <v>367</v>
-      </c>
-      <c r="E187" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B189" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C189" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D189" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E189" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B190" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C190" t="s">
+        <v>293</v>
+      </c>
+      <c r="D190" t="s">
+        <v>295</v>
+      </c>
+      <c r="E190" t="s">
         <v>297</v>
-      </c>
-      <c r="D190" t="s">
-        <v>299</v>
-      </c>
-      <c r="E190" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B191" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C191" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D191" t="s">
-        <v>303</v>
+        <v>426</v>
       </c>
       <c r="E191" t="s">
-        <v>305</v>
+        <v>438</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B192" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C192" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D192" t="s">
-        <v>304</v>
+        <v>427</v>
       </c>
       <c r="E192" t="s">
-        <v>306</v>
+        <v>439</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B193" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C193" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D193" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="E193" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B194" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C194" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D194" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E194" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B195" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C195" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D195" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E195" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B196" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C196" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D196" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E196" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B197" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C197" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D197" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E197" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B198" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C198" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D198" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="E198" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4729,16 +4756,16 @@
         <v>10</v>
       </c>
       <c r="B200" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C200" t="s">
-        <v>370</v>
+        <v>312</v>
       </c>
       <c r="D200" t="s">
-        <v>371</v>
+        <v>313</v>
       </c>
       <c r="E200" t="s">
-        <v>375</v>
+        <v>315</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4746,16 +4773,16 @@
         <v>10</v>
       </c>
       <c r="B201" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C201" t="s">
-        <v>370</v>
+        <v>312</v>
       </c>
       <c r="D201" t="s">
-        <v>372</v>
+        <v>314</v>
       </c>
       <c r="E201" t="s">
-        <v>376</v>
+        <v>316</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4763,16 +4790,16 @@
         <v>10</v>
       </c>
       <c r="B202" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C202" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D202" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="E202" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4780,16 +4807,50 @@
         <v>10</v>
       </c>
       <c r="B203" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C203" t="s">
+        <v>366</v>
+      </c>
+      <c r="D203" t="s">
+        <v>368</v>
+      </c>
+      <c r="E203" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>10</v>
+      </c>
+      <c r="B204" t="s">
+        <v>108</v>
+      </c>
+      <c r="C204" t="s">
+        <v>366</v>
+      </c>
+      <c r="D204" t="s">
+        <v>369</v>
+      </c>
+      <c r="E204" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>10</v>
+      </c>
+      <c r="B205" t="s">
+        <v>109</v>
+      </c>
+      <c r="C205" t="s">
+        <v>366</v>
+      </c>
+      <c r="D205" t="s">
         <v>370</v>
       </c>
-      <c r="D203" t="s">
+      <c r="E205" t="s">
         <v>374</v>
-      </c>
-      <c r="E203" t="s">
-        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>